<commit_message>
implement only for output_image
</commit_message>
<xml_diff>
--- a/figures2/result.xlsx
+++ b/figures2/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sakakibara\monte-carlo-ray-tracer_approx\figures2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E17B6E2-751D-44A7-9C06-F04B8F4450CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B57985-9BCD-46A4-9DB2-E75336E1E3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3845,37 +3845,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3898,7 +3868,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="808080"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3909,11 +3879,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="808080"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="808080"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4015,7 +3985,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="8054FF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4026,11 +3996,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="8054FF"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:srgbClr val="8054FF"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4132,7 +4102,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF2580"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4143,11 +4113,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF2580"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:srgbClr val="FF2580"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4265,6 +4235,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>近似積極度</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4327,6 +4352,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>MSE</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -18099,8 +18180,8 @@
       <xdr:rowOff>2381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>648973</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>653735</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>117956</xdr:rowOff>
     </xdr:to>
@@ -19641,8 +19722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC53CF9-F476-46BF-844B-A201D5CD8083}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -20185,8 +20266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6519B477-C4AB-467B-9B48-9C9ED35D0024}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>

</xml_diff>